<commit_message>
chore: publish carecommunication IG 4.0.3
</commit_message>
<xml_diff>
--- a/ig/carecommunication/StructureDefinition-medcom-careCommunication-communication.xlsx
+++ b/ig/carecommunication/StructureDefinition-medcom-careCommunication-communication.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>4.0.2</t>
+    <t>4.0.3</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-11-07T14:20:03+01:00</t>
+    <t>2025-05-23T11:28:08+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1994,17 +1994,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="56.71875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="44.55078125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="14.015625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="5.90234375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.69921875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="57.98046875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="45.58203125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="14.21875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="39.9140625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="6.77734375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.9453125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="5.4296875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="16.27734375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="13.26171875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="165.29296875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="166.4140625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -2013,25 +2013,25 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="38.8125" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="15.71484375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="16.08984375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="17.078125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="16.3125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="95.56640625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="85.18359375" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="40.0390625" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="14.98828125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="12.3046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="34.94921875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="9.87890625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="38.2265625" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="17.171875" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.65625" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="18.859375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="98.375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="85.26953125" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="42.03515625" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="17.21484375" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="14.4140625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="35.859375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="10.5546875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="11.0390625" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="48.1484375" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="32.84375" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="99.69140625" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="50.6484375" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="36.91796875" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="102.6171875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
chore: publish carecommunication IG 5.0.1
</commit_message>
<xml_diff>
--- a/ig/carecommunication/StructureDefinition-medcom-careCommunication-communication.xlsx
+++ b/ig/carecommunication/StructureDefinition-medcom-careCommunication-communication.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>5.0.0</t>
+    <t>5.0.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-27T14:45:58+00:00</t>
+    <t>2025-10-29T10:10:10+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -534,7 +534,7 @@
     <t>sender</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-sender-extension|3.0.0}
+    <t xml:space="preserve">Extension {http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-sender-extension|3.0.1}
 </t>
   </si>
   <si>
@@ -896,7 +896,7 @@
     <t>There may be multiple axes of categorization and one communication may serve multiple purposes.</t>
   </si>
   <si>
-    <t>http://medcomfhir.dk/ig/terminology/ValueSet/medcom-careCommunication-categories|1.8.1</t>
+    <t>http://medcomfhir.dk/ig/terminology/ValueSet/medcom-careCommunication-categories|1.9.0</t>
   </si>
   <si>
     <t>FiveWs.class</t>
@@ -1103,7 +1103,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-patient|3.0.0) &lt;&lt;bundled&gt;&gt;
+    <t xml:space="preserve">Reference(http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-patient|3.0.1) &lt;&lt;bundled&gt;&gt;
 </t>
   </si>
   <si>
@@ -1167,7 +1167,7 @@
     <t>Communication.encounter</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-encounter|3.0.0) &lt;&lt;bundled&gt;&gt;
+    <t xml:space="preserve">Reference(http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-encounter|3.0.1) &lt;&lt;bundled&gt;&gt;
 </t>
   </si>
   <si>
@@ -1217,7 +1217,7 @@
     <t>Communication.recipient</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-practitionerrole|3.0.0|http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-careteam|3.0.0) &lt;&lt;bundled&gt;&gt;
+    <t xml:space="preserve">Reference(http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-practitionerrole|3.0.1|http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-careteam|3.0.1) &lt;&lt;bundled&gt;&gt;
 </t>
   </si>
   <si>
@@ -1321,7 +1321,7 @@
     <t>date</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-datetime-extension|3.0.0}
+    <t xml:space="preserve">Extension {http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-datetime-extension|3.0.1}
 </t>
   </si>
   <si>
@@ -1337,7 +1337,7 @@
     <t>author</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-practitioner-extension|3.0.0}
+    <t xml:space="preserve">Extension {http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-practitioner-extension|3.0.1}
 </t>
   </si>
   <si>
@@ -1353,7 +1353,7 @@
     <t>authorContact</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-contact-extension|3.0.0}
+    <t xml:space="preserve">Extension {http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-contact-extension|3.0.1}
 </t>
   </si>
   <si>
@@ -1369,7 +1369,7 @@
     <t>identifier</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-identifier-extension|3.0.0}
+    <t xml:space="preserve">Extension {http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-identifier-extension|3.0.1}
 </t>
   </si>
   <si>

</xml_diff>

<commit_message>
chore: publish carecommunication IG 5.0.1 (#49)
Co-authored-by: sksMedcom <sksMedcom@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ig/carecommunication/StructureDefinition-medcom-careCommunication-communication.xlsx
+++ b/ig/carecommunication/StructureDefinition-medcom-careCommunication-communication.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>5.0.0</t>
+    <t>5.0.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-27T14:45:58+00:00</t>
+    <t>2025-10-29T10:10:10+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -534,7 +534,7 @@
     <t>sender</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-sender-extension|3.0.0}
+    <t xml:space="preserve">Extension {http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-sender-extension|3.0.1}
 </t>
   </si>
   <si>
@@ -896,7 +896,7 @@
     <t>There may be multiple axes of categorization and one communication may serve multiple purposes.</t>
   </si>
   <si>
-    <t>http://medcomfhir.dk/ig/terminology/ValueSet/medcom-careCommunication-categories|1.8.1</t>
+    <t>http://medcomfhir.dk/ig/terminology/ValueSet/medcom-careCommunication-categories|1.9.0</t>
   </si>
   <si>
     <t>FiveWs.class</t>
@@ -1103,7 +1103,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-patient|3.0.0) &lt;&lt;bundled&gt;&gt;
+    <t xml:space="preserve">Reference(http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-patient|3.0.1) &lt;&lt;bundled&gt;&gt;
 </t>
   </si>
   <si>
@@ -1167,7 +1167,7 @@
     <t>Communication.encounter</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-encounter|3.0.0) &lt;&lt;bundled&gt;&gt;
+    <t xml:space="preserve">Reference(http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-encounter|3.0.1) &lt;&lt;bundled&gt;&gt;
 </t>
   </si>
   <si>
@@ -1217,7 +1217,7 @@
     <t>Communication.recipient</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-practitionerrole|3.0.0|http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-careteam|3.0.0) &lt;&lt;bundled&gt;&gt;
+    <t xml:space="preserve">Reference(http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-practitionerrole|3.0.1|http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-careteam|3.0.1) &lt;&lt;bundled&gt;&gt;
 </t>
   </si>
   <si>
@@ -1321,7 +1321,7 @@
     <t>date</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-datetime-extension|3.0.0}
+    <t xml:space="preserve">Extension {http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-datetime-extension|3.0.1}
 </t>
   </si>
   <si>
@@ -1337,7 +1337,7 @@
     <t>author</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-practitioner-extension|3.0.0}
+    <t xml:space="preserve">Extension {http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-practitioner-extension|3.0.1}
 </t>
   </si>
   <si>
@@ -1353,7 +1353,7 @@
     <t>authorContact</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-contact-extension|3.0.0}
+    <t xml:space="preserve">Extension {http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-contact-extension|3.0.1}
 </t>
   </si>
   <si>
@@ -1369,7 +1369,7 @@
     <t>identifier</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-identifier-extension|3.0.0}
+    <t xml:space="preserve">Extension {http://medcomfhir.dk/ig/core/StructureDefinition/medcom-core-identifier-extension|3.0.1}
 </t>
   </si>
   <si>

</xml_diff>